<commit_message>
Added a repetition assignment based on wildcard count.
</commit_message>
<xml_diff>
--- a/projectfiles/data/Variable Dictionary.xlsx
+++ b/projectfiles/data/Variable Dictionary.xlsx
@@ -5,18 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HAL9000\Desktop\kod\Automator\Automator 2.0\projectfiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HAL9000\Desktop\kod\Automator\Automator 2.0\projectfiles\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE0F9E6-11AB-44EC-86F8-024FF2F884B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0175579-1A16-4595-89E0-5947995DB9B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1932" yWindow="1932" windowWidth="14916" windowHeight="10428" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8124" yWindow="1932" windowWidth="14916" windowHeight="10428" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -357,7 +361,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection sqref="A1:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added: Repeat commands based on the wildcard count, search an copy files, use full filenames as variables or wildcards.
</commit_message>
<xml_diff>
--- a/projectfiles/data/Variable Dictionary.xlsx
+++ b/projectfiles/data/Variable Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HAL9000\Desktop\kod\Automator\Automator 2.0\projectfiles\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0175579-1A16-4595-89E0-5947995DB9B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{926B8276-F973-43C5-9A86-F3FCDF9DBB4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8124" yWindow="1932" windowWidth="14916" windowHeight="10428" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="14916" windowHeight="11808" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,68 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+  <si>
+    <t>brave</t>
+  </si>
+  <si>
+    <t>history</t>
+  </si>
+  <si>
+    <t>strong</t>
+  </si>
+  <si>
+    <t>book</t>
+  </si>
+  <si>
+    <t>coward</t>
+  </si>
+  <si>
+    <t>read</t>
+  </si>
+  <si>
+    <t>fat</t>
+  </si>
+  <si>
+    <t>write</t>
+  </si>
+  <si>
+    <t>ugly</t>
+  </si>
+  <si>
+    <t>listen</t>
+  </si>
+  <si>
+    <t>handsome</t>
+  </si>
+  <si>
+    <t>face</t>
+  </si>
+  <si>
+    <t>horror</t>
+  </si>
+  <si>
+    <t>look</t>
+  </si>
+  <si>
+    <t>fantasy</t>
+  </si>
+  <si>
+    <t>screen</t>
+  </si>
+  <si>
+    <t>science fiction</t>
+  </si>
+  <si>
+    <t>computer</t>
+  </si>
+  <si>
+    <t>comedy</t>
+  </si>
+  <si>
+    <t>head</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -358,14 +419,95 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F8"/>
+      <selection sqref="A1:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>